<commit_message>
sudah penyesuaian tabel namun masih bermasalah di lokasi absen dan jam kerja
</commit_message>
<xml_diff>
--- a/public/importexcel/data karyawan.xlsx
+++ b/public/importexcel/data karyawan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onedrive\OneDrive - Bina Nusantara\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D551A3-7C6D-48BD-A752-B316165D66F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207C8761-2093-4628-AB90-2A2E5881EBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8C9AEB27-2046-4AC1-B53F-C22D4219FAD0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>No</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Divisi</t>
   </si>
   <si>
-    <t>Anak Perusahaan</t>
-  </si>
-  <si>
     <t>Slamet</t>
   </si>
   <si>
@@ -77,32 +74,119 @@
     <t>Staff HRD</t>
   </si>
   <si>
-    <t>Keuangan</t>
-  </si>
-  <si>
-    <t>'08687976865</t>
-  </si>
-  <si>
     <t>HRD</t>
   </si>
   <si>
-    <t>Ulala</t>
-  </si>
-  <si>
     <t>CLC</t>
   </si>
   <si>
     <t>FNC</t>
   </si>
   <si>
-    <t>MKR01</t>
+    <t>Staff Griya Sehat</t>
+  </si>
+  <si>
+    <t>Staff Keuangan</t>
+  </si>
+  <si>
+    <t>08687976865</t>
+  </si>
+  <si>
+    <t>L001</t>
+  </si>
+  <si>
+    <t>L002</t>
+  </si>
+  <si>
+    <t>Sienna</t>
+  </si>
+  <si>
+    <t>Raissa</t>
+  </si>
+  <si>
+    <t>Roni</t>
+  </si>
+  <si>
+    <t>Riko</t>
+  </si>
+  <si>
+    <t>Riki</t>
+  </si>
+  <si>
+    <t>Marsya</t>
+  </si>
+  <si>
+    <t>Widi</t>
+  </si>
+  <si>
+    <t>Cindi</t>
+  </si>
+  <si>
+    <t>Rena</t>
+  </si>
+  <si>
+    <t>Rani</t>
+  </si>
+  <si>
+    <t>Staff IT</t>
+  </si>
+  <si>
+    <t>Office Boy</t>
+  </si>
+  <si>
+    <t>Staff LPM</t>
+  </si>
+  <si>
+    <t>Ketua STAB</t>
+  </si>
+  <si>
+    <t>Kaprodi</t>
+  </si>
+  <si>
+    <t>OB</t>
+  </si>
+  <si>
+    <t>Kepala Tendik</t>
+  </si>
+  <si>
+    <t>Staff Tendik</t>
+  </si>
+  <si>
+    <t>08687976864</t>
+  </si>
+  <si>
+    <t>08687976843</t>
+  </si>
+  <si>
+    <t>08687976866</t>
+  </si>
+  <si>
+    <t>08687976869</t>
+  </si>
+  <si>
+    <t>Nama Anper</t>
+  </si>
+  <si>
+    <t>DSN01</t>
+  </si>
+  <si>
+    <t>DSN02</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>LPM</t>
+  </si>
+  <si>
+    <t>TK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +198,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -160,12 +250,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -482,144 +578,386 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB2E317D-F07C-4BFF-81D3-A0A091D727EC}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
     <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="26.5546875" customWidth="1"/>
     <col min="8" max="8" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="H1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>111050</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>111051</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>111052</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>111053</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>111054</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>111055</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>111056</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>111057</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>111058</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>111059</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>111060</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>111061</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>111062</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>111063</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>